<commit_message>
Update Saldo Simpanan dan Saldo Pinjaman
</commit_message>
<xml_diff>
--- a/assets/template/Contoh_Format_Saldo.xlsx
+++ b/assets/template/Contoh_Format_Saldo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\inkopkar\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531CE4D3-FE6D-472E-893B-8FD8D1A1BD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D94275-95BC-487C-B758-456E16CF39B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2E8CD1E3-45E7-4754-8C58-5E9B6364AB8C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Nomor Anggota</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>IURAN BULAN JUNI 2025</t>
   </si>
 </sst>
 </file>
@@ -500,23 +506,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0B6173-9C9B-4B37-B0E3-EBD30C0093EF}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -524,37 +530,51 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
         <v>500000</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="4">
         <v>50000</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>